<commit_message>
update eval data of LLM
</commit_message>
<xml_diff>
--- a/LLM-eval/file/TestPlan.xlsx
+++ b/LLM-eval/file/TestPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17680"/>
+    <workbookView windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>序号</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>用例集</t>
+  </si>
+  <si>
+    <t>描述</t>
   </si>
   <si>
     <t>总结</t>
@@ -101,6 +104,9 @@
     <t>file/suite/continuousChat1.xlsx</t>
   </si>
   <si>
+    <t>工具调用：普通crud</t>
+  </si>
+  <si>
     <t xml:space="preserve"># 测试结果汇总
 ## 总用例数：50，平均分：9.9
 </t>
@@ -119,7 +125,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,13 +135,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -238,14 +237,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -593,79 +584,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -677,7 +668,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -689,7 +680,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -701,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -713,7 +704,7 @@
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -725,7 +716,7 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1070,10 +1061,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
@@ -1083,11 +1074,11 @@
     <col min="5" max="5" width="61.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="49.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.25" style="1" customWidth="1"/>
-    <col min="9" max="12" width="9" style="1"/>
+    <col min="8" max="9" width="21.25" style="1" customWidth="1"/>
+    <col min="10" max="13" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1118,37 +1109,43 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" ht="409.5" spans="1:10">
+    <row r="2" ht="409.5" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>